<commit_message>
add dns and up
</commit_message>
<xml_diff>
--- a/spec/ark3530_single_specs.xlsx
+++ b/spec/ark3530_single_specs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="466" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="465" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Platform" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="127">
   <si>
     <t>Catalog</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Database</t>
   </si>
   <si>
-    <t>MongoDB, CHART: mongodb-replicaset-3.5.6, APP: 3.6</t>
-  </si>
-  <si>
     <t>IoTHub</t>
   </si>
   <si>
@@ -52,10 +49,6 @@
   </si>
   <si>
     <t>Memory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PostgreSQL, CHART: stolon-0.4.3, APP: 9.6</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -111,18 +104,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Version/Spec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>quay.io/external_storage/rbd-provisioner:v1.1.0-k8s1.10</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Kubernetes v-1.10.7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Kubernetes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -131,26 +116,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RabbitMQ, CHART: rabbitmq-ha-1.10.0, APP: 3.7.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Minio, CHART: minio-1.6.3, APP: RELEASE.2018-08-25T01-56-38Z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prometheus v-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Prometheus</t>
   </si>
   <si>
     <t>Monitor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ingress, CHART: nginx-ingress 0.28.2, nginx-ingress-controller: 0.19.0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -246,14 +215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>minio/minio:RELEASE.2018-08-25T01-56-38Z</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Grafana v-5.2.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PV(G)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -262,10 +223,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>es-minio-1.6.3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Note</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -430,10 +387,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Introduction of Edge Server</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DNS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -467,11 +420,6 @@
   </si>
   <si>
     <t>Modify Domain Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. Change all TCP NodePorts to Nginx Ports
-2. Mongo Exporter (Evelyn)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -545,11 +493,29 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TODO (Alex)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Containerd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minio-2.3.4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minio/minio:RELEASE.2018-12-06T01-27-43Z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Change all TCP NodePorts to Nginx Ports
+2. Mongo Exporter (Evelyn)
+3. recycling mechanism (Evelyn)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Introduction of Edge Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1178,10 +1144,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,21 +1155,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1217,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1233,14 +1199,13 @@
     <col min="6" max="6" width="21.375" style="12" customWidth="1"/>
     <col min="7" max="7" width="13.75" style="12" customWidth="1"/>
     <col min="8" max="8" width="26.75" style="12" customWidth="1"/>
-    <col min="9" max="9" width="27.5" style="12" customWidth="1"/>
-    <col min="10" max="12" width="18.625" style="12" customWidth="1"/>
-    <col min="13" max="13" width="16" style="12" customWidth="1"/>
-    <col min="14" max="14" width="71.5" style="12" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="12"/>
+    <col min="9" max="11" width="18.625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="16" style="12" customWidth="1"/>
+    <col min="13" max="13" width="71.5" style="12" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1248,168 +1213,159 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="21">
         <v>1</v>
       </c>
       <c r="H2" s="17"/>
-      <c r="I2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="I2" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="17"/>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="23"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="2">
         <v>3</v>
       </c>
       <c r="H4" s="17"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I4" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="25"/>
       <c r="C5" s="6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G5" s="2">
         <v>0.25</v>
       </c>
       <c r="H5" s="17"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="17"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G6" s="2">
         <v>6</v>
@@ -1417,33 +1373,30 @@
       <c r="H6" s="2">
         <v>1433.6</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="I6" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="17"/>
       <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="25"/>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G7" s="2">
         <v>0.5</v>
@@ -1451,35 +1404,32 @@
       <c r="H7" s="2">
         <v>8</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="I7" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G8" s="2">
         <v>6</v>
@@ -1487,305 +1437,290 @@
       <c r="H8" s="2">
         <v>32</v>
       </c>
-      <c r="I8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>77</v>
+      <c r="I8" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G9" s="2">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="H9" s="2">
         <v>10</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>32</v>
+      <c r="I9" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G10" s="2">
         <v>1.5</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="G11" s="2">
         <v>0.25</v>
       </c>
       <c r="H11" s="17"/>
-      <c r="I11" s="6" t="s">
-        <v>61</v>
+      <c r="I11" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G12" s="2">
         <v>1</v>
       </c>
       <c r="H12" s="17"/>
-      <c r="I12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G13" s="2">
         <v>0.5</v>
       </c>
       <c r="H13" s="17"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="I13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="17"/>
       <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
       <c r="H14" s="17"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="15" t="s">
-        <v>77</v>
+      <c r="I14" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="M14" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="26"/>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D15" s="22"/>
       <c r="E15" s="15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
       <c r="H15" s="17"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I15" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="17"/>
       <c r="K15" s="17"/>
       <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="26"/>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="15" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G16" s="2">
         <v>0.5</v>
       </c>
       <c r="H16" s="17"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="I16" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="2"/>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G17" s="2">
         <f>SUM(G2:G16)</f>
-        <v>24.5</v>
+        <v>23.75</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H2:H16)</f>
@@ -1814,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1834,74 +1769,74 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="7" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="25" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F5" s="20"/>
     </row>
@@ -1909,11 +1844,11 @@
       <c r="A6" s="24"/>
       <c r="B6" s="26"/>
       <c r="C6" s="7" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="F6" s="20"/>
     </row>
@@ -1921,7 +1856,7 @@
       <c r="A7" s="24"/>
       <c r="B7" s="26"/>
       <c r="C7" s="25" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
@@ -1971,7 +1906,7 @@
       <c r="A13" s="24"/>
       <c r="B13" s="26"/>
       <c r="C13" s="7" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1981,13 +1916,13 @@
       <c r="A14" s="24"/>
       <c r="B14" s="26"/>
       <c r="C14" s="18" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F14" s="20"/>
     </row>
@@ -1995,7 +1930,7 @@
       <c r="A15" s="24"/>
       <c r="B15" s="26"/>
       <c r="C15" s="7" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -2005,13 +1940,13 @@
       <c r="A16" s="24"/>
       <c r="B16" s="26"/>
       <c r="C16" s="25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="F16" s="20"/>
     </row>
@@ -2020,10 +1955,10 @@
       <c r="B17" s="26"/>
       <c r="C17" s="29"/>
       <c r="D17" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="F17" s="20"/>
     </row>
@@ -2032,10 +1967,10 @@
       <c r="B18" s="26"/>
       <c r="C18" s="29"/>
       <c r="D18" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F18" s="20"/>
     </row>
@@ -2044,20 +1979,20 @@
       <c r="B19" s="26"/>
       <c r="C19" s="29"/>
       <c r="D19" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -2066,10 +2001,10 @@
     <row r="21" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="21" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -2079,7 +2014,7 @@
       <c r="A22" s="24"/>
       <c r="B22" s="28"/>
       <c r="C22" s="2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -2089,7 +2024,7 @@
       <c r="A23" s="24"/>
       <c r="B23" s="23"/>
       <c r="C23" s="2" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2098,10 +2033,10 @@
     <row r="24" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="13" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -2110,7 +2045,7 @@
     <row r="25" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="13" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2120,7 +2055,7 @@
     <row r="26" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="13" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2129,7 +2064,7 @@
     </row>
     <row r="27" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -2139,7 +2074,7 @@
     </row>
     <row r="28" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="B28" s="20"/>
       <c r="C28" s="20"/>

</xml_diff>